<commit_message>
Finished parameter estimates, started on quantiles
</commit_message>
<xml_diff>
--- a/Data/C_BIC_and_AIC_new.xlsx
+++ b/Data/C_BIC_and_AIC_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\Documents\GitHub\Master-Thesis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A349F3F-4BCC-4CBD-BA70-3B43A8D4DF09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEE1FD8-39FF-4C42-92DB-691A319F0A90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{8B4AF45F-4553-42B7-ADB3-4705C4B01884}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="9">
   <si>
     <t>BIC</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>df</t>
-  </si>
-  <si>
-    <t>**</t>
   </si>
   <si>
     <t>Summer</t>
@@ -417,7 +414,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -427,18 +424,18 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -453,7 +450,7 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -476,10 +473,10 @@
         <v>762.32</v>
       </c>
       <c r="C3">
-        <v>561.61</v>
+        <v>558.97</v>
       </c>
       <c r="D3">
-        <v>428.44</v>
+        <v>445.39</v>
       </c>
       <c r="E3">
         <v>331.65</v>
@@ -488,19 +485,19 @@
         <v>2</v>
       </c>
       <c r="H3">
-        <f>B3</f>
+        <f t="shared" ref="H3:K4" si="0">B3</f>
         <v>762.32</v>
       </c>
       <c r="I3">
-        <f>C3</f>
-        <v>561.61</v>
+        <f t="shared" si="0"/>
+        <v>558.97</v>
       </c>
       <c r="J3">
-        <f>D3</f>
-        <v>428.44</v>
+        <f t="shared" si="0"/>
+        <v>445.39</v>
       </c>
       <c r="K3">
-        <f>E3</f>
+        <f t="shared" si="0"/>
         <v>331.65</v>
       </c>
     </row>
@@ -512,10 +509,10 @@
         <v>75.44</v>
       </c>
       <c r="C4">
-        <v>353.07</v>
+        <v>174.37</v>
       </c>
       <c r="D4">
-        <v>230.56</v>
+        <v>215.91</v>
       </c>
       <c r="E4">
         <v>215.5</v>
@@ -524,19 +521,19 @@
         <v>3</v>
       </c>
       <c r="H4">
-        <f>B4</f>
+        <f t="shared" si="0"/>
         <v>75.44</v>
       </c>
       <c r="I4">
-        <f>C4</f>
-        <v>353.07</v>
+        <f t="shared" si="0"/>
+        <v>174.37</v>
       </c>
       <c r="J4">
-        <f>D4</f>
-        <v>230.56</v>
+        <f t="shared" si="0"/>
+        <v>215.91</v>
       </c>
       <c r="K4">
-        <f>E4</f>
+        <f t="shared" si="0"/>
         <v>215.5</v>
       </c>
     </row>
@@ -550,11 +547,11 @@
       </c>
       <c r="C5">
         <f>C3*2+C4*LN(24*24*2)</f>
-        <v>3612.1004068021984</v>
+        <v>2347.1185666697802</v>
       </c>
       <c r="D5">
         <f>D3*2+D4*LN(24*24*2)</f>
-        <v>2482.156196199946</v>
+        <v>2412.7846127755474</v>
       </c>
       <c r="E5">
         <f>E3*2+E4*LN(24*24*2)</f>
@@ -568,24 +565,24 @@
         <v>1675.52</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:K5" si="0">I3*2+I4*2</f>
-        <v>1829.3600000000001</v>
+        <f t="shared" ref="I5:K5" si="1">I3*2+I4*2</f>
+        <v>1466.68</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
-        <v>1318</v>
+        <f t="shared" si="1"/>
+        <v>1322.6</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1094.3</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -599,26 +596,29 @@
         <v>737.69</v>
       </c>
       <c r="D7">
-        <v>613.53</v>
+        <v>666.18</v>
+      </c>
+      <c r="E7">
+        <v>499.69</v>
       </c>
       <c r="G7" t="s">
         <v>2</v>
       </c>
       <c r="H7">
-        <f>B7</f>
+        <f t="shared" ref="H7:K8" si="2">B7</f>
         <v>976.14</v>
       </c>
       <c r="I7">
-        <f>C7</f>
+        <f t="shared" si="2"/>
         <v>737.69</v>
       </c>
       <c r="J7">
-        <f>D7</f>
-        <v>613.53</v>
+        <f t="shared" si="2"/>
+        <v>666.18</v>
       </c>
       <c r="K7">
-        <f>E7</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>499.69</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -632,26 +632,29 @@
         <v>104.51</v>
       </c>
       <c r="D8">
-        <v>149.13</v>
+        <v>167.24</v>
+      </c>
+      <c r="E8">
+        <v>226.4</v>
       </c>
       <c r="G8" t="s">
         <v>3</v>
       </c>
       <c r="H8">
-        <f>B8</f>
+        <f t="shared" si="2"/>
         <v>79.84</v>
       </c>
       <c r="I8">
-        <f>C8</f>
+        <f t="shared" si="2"/>
         <v>104.51</v>
       </c>
       <c r="J8">
-        <f>D8</f>
-        <v>149.13</v>
+        <f t="shared" si="2"/>
+        <v>167.24</v>
       </c>
       <c r="K8">
-        <f>E8</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>226.4</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -668,11 +671,11 @@
       </c>
       <c r="D9">
         <f>D7*2+D8*LN(24*24*2)</f>
-        <v>2278.3153744764832</v>
+        <v>2511.2773796516262</v>
       </c>
       <c r="E9">
         <f>E7*2+E8*LN(24*24*2)</f>
-        <v>0</v>
+        <v>2595.3312960603216</v>
       </c>
       <c r="G9" t="s">
         <v>1</v>
@@ -682,37 +685,29 @@
         <v>2111.96</v>
       </c>
       <c r="I9">
-        <f t="shared" ref="I9:K9" si="1">I7*2+I8*2</f>
+        <f t="shared" ref="I9:K9" si="3">I7*2+I8*2</f>
         <v>1684.4</v>
       </c>
       <c r="J9">
-        <f t="shared" si="1"/>
-        <v>1525.32</v>
+        <f t="shared" si="3"/>
+        <v>1666.84</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J10" t="s">
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>1452.18</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -727,7 +722,7 @@
         <v>5</v>
       </c>
       <c r="G14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -762,19 +757,19 @@
         <v>2</v>
       </c>
       <c r="H15">
-        <f>B15</f>
+        <f t="shared" ref="H15:K16" si="4">B15</f>
         <v>-902.09</v>
       </c>
       <c r="I15">
-        <f>C15</f>
+        <f t="shared" si="4"/>
         <v>-1245.75</v>
       </c>
       <c r="J15">
-        <f>D15</f>
+        <f t="shared" si="4"/>
         <v>-1561</v>
       </c>
       <c r="K15">
-        <f>E15</f>
+        <f t="shared" si="4"/>
         <v>-1773</v>
       </c>
     </row>
@@ -786,7 +781,7 @@
         <v>16.59</v>
       </c>
       <c r="C16">
-        <v>46.53</v>
+        <v>57.22</v>
       </c>
       <c r="D16">
         <v>30.5</v>
@@ -798,19 +793,19 @@
         <v>3</v>
       </c>
       <c r="H16">
-        <f>B16</f>
+        <f t="shared" si="4"/>
         <v>16.59</v>
       </c>
       <c r="I16">
-        <f>C16</f>
-        <v>46.53</v>
+        <f t="shared" si="4"/>
+        <v>57.22</v>
       </c>
       <c r="J16">
-        <f>D16</f>
+        <f t="shared" si="4"/>
         <v>30.5</v>
       </c>
       <c r="K16">
-        <f>E16</f>
+        <f t="shared" si="4"/>
         <v>33.840000000000003</v>
       </c>
     </row>
@@ -824,7 +819,7 @@
       </c>
       <c r="C17">
         <f>C15*2+C16*LN(24*24*2)</f>
-        <v>-2163.4981722363659</v>
+        <v>-2088.1416379833408</v>
       </c>
       <c r="D17">
         <f>D15*2+D16*LN(24*24*2)</f>
@@ -842,24 +837,24 @@
         <v>-1771</v>
       </c>
       <c r="I17">
-        <f t="shared" ref="I17:K17" si="2">I15*2+I16*2</f>
-        <v>-2398.44</v>
+        <f t="shared" ref="I17:K17" si="5">I15*2+I16*2</f>
+        <v>-2377.06</v>
       </c>
       <c r="J17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-3061</v>
       </c>
       <c r="K17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-3478.32</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -873,26 +868,29 @@
         <v>-1279.6500000000001</v>
       </c>
       <c r="D19">
-        <v>-1557.67</v>
+        <v>-1552.77</v>
+      </c>
+      <c r="E19">
+        <v>-1792.03</v>
       </c>
       <c r="G19" t="s">
         <v>2</v>
       </c>
       <c r="H19">
-        <f>B19</f>
+        <f t="shared" ref="H19:K20" si="6">B19</f>
         <v>-923.2</v>
       </c>
       <c r="I19">
-        <f>C19</f>
+        <f t="shared" si="6"/>
         <v>-1279.6500000000001</v>
       </c>
       <c r="J19">
-        <f>D19</f>
-        <v>-1557.67</v>
+        <f t="shared" si="6"/>
+        <v>-1552.77</v>
       </c>
       <c r="K19">
-        <f>E19</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>-1792.03</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -906,26 +904,29 @@
         <v>27.07</v>
       </c>
       <c r="D20">
-        <v>-5.17</v>
+        <v>20.88</v>
+      </c>
+      <c r="E20">
+        <v>23.09</v>
       </c>
       <c r="G20" t="s">
         <v>3</v>
       </c>
       <c r="H20">
-        <f>B20</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="I20">
-        <f>C20</f>
+        <f t="shared" si="6"/>
         <v>27.07</v>
       </c>
       <c r="J20">
-        <f>D20</f>
-        <v>-5.17</v>
+        <f t="shared" si="6"/>
+        <v>20.88</v>
       </c>
       <c r="K20">
-        <f>E20</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>23.09</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -942,11 +943,11 @@
       </c>
       <c r="D21">
         <f>D19*2+D20*LN(24*24*2)</f>
-        <v>-3151.7846475292927</v>
+        <v>-2958.3515589145782</v>
       </c>
       <c r="E21">
         <f>E19*2+E20*LN(24*24*2)</f>
-        <v>0</v>
+        <v>-3421.2927057154025</v>
       </c>
       <c r="G21" t="s">
         <v>1</v>
@@ -956,29 +957,29 @@
         <v>-1830.4</v>
       </c>
       <c r="I21">
-        <f t="shared" ref="I21:K21" si="3">I19*2+I20*2</f>
+        <f t="shared" ref="I21:K21" si="7">I19*2+I20*2</f>
         <v>-2505.1600000000003</v>
       </c>
       <c r="J21">
-        <f t="shared" si="3"/>
-        <v>-3125.6800000000003</v>
+        <f t="shared" si="7"/>
+        <v>-3063.7799999999997</v>
       </c>
       <c r="K21">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>-3537.88</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -993,7 +994,7 @@
         <v>5</v>
       </c>
       <c r="G26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H26">
         <v>2</v>
@@ -1018,11 +1019,11 @@
       </c>
       <c r="C27">
         <f>C3</f>
-        <v>561.61</v>
+        <v>558.97</v>
       </c>
       <c r="D27">
         <f>D3</f>
-        <v>428.44</v>
+        <v>445.39</v>
       </c>
       <c r="E27">
         <f>E3</f>
@@ -1032,19 +1033,19 @@
         <v>2</v>
       </c>
       <c r="H27">
-        <f>B27</f>
+        <f t="shared" ref="H27:K28" si="8">B27</f>
         <v>762.32</v>
       </c>
       <c r="I27">
-        <f>C27</f>
-        <v>561.61</v>
+        <f t="shared" si="8"/>
+        <v>558.97</v>
       </c>
       <c r="J27">
-        <f>D27</f>
-        <v>428.44</v>
+        <f t="shared" si="8"/>
+        <v>445.39</v>
       </c>
       <c r="K27">
-        <f>E27</f>
+        <f t="shared" si="8"/>
         <v>331.65</v>
       </c>
     </row>
@@ -1058,7 +1059,7 @@
       </c>
       <c r="C28">
         <f>C16</f>
-        <v>46.53</v>
+        <v>57.22</v>
       </c>
       <c r="D28">
         <f>D16</f>
@@ -1072,19 +1073,19 @@
         <v>3</v>
       </c>
       <c r="H28">
-        <f>B28</f>
+        <f t="shared" si="8"/>
         <v>16.59</v>
       </c>
       <c r="I28">
-        <f>C28</f>
-        <v>46.53</v>
+        <f t="shared" si="8"/>
+        <v>57.22</v>
       </c>
       <c r="J28">
-        <f>D28</f>
+        <f t="shared" si="8"/>
         <v>30.5</v>
       </c>
       <c r="K28">
-        <f>E28</f>
+        <f t="shared" si="8"/>
         <v>33.840000000000003</v>
       </c>
     </row>
@@ -1098,11 +1099,11 @@
       </c>
       <c r="C29">
         <f>C27*2+C28*LN(24*24*2)</f>
-        <v>1451.2218277636341</v>
+        <v>1521.298362016659</v>
       </c>
       <c r="D29">
         <f>D27*2+D28*LN(24*24*2)</f>
-        <v>1071.882272658303</v>
+        <v>1105.7822726583031</v>
       </c>
       <c r="E29">
         <f>E27*2+E28*LN(24*24*2)</f>
@@ -1116,24 +1117,24 @@
         <v>1557.8200000000002</v>
       </c>
       <c r="I29">
-        <f t="shared" ref="I29:K29" si="4">I27*2+I28*2</f>
-        <v>1216.28</v>
+        <f t="shared" ref="I29:K29" si="9">I27*2+I28*2</f>
+        <v>1232.3800000000001</v>
       </c>
       <c r="J29">
-        <f t="shared" si="4"/>
-        <v>917.88</v>
+        <f t="shared" si="9"/>
+        <v>951.78</v>
       </c>
       <c r="K29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>730.98</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1145,35 +1146,35 @@
         <v>976.14</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:E31" si="5">C7</f>
+        <f t="shared" ref="C31:E31" si="10">C7</f>
         <v>737.69</v>
       </c>
       <c r="D31">
-        <f t="shared" si="5"/>
-        <v>613.53</v>
+        <f t="shared" si="10"/>
+        <v>666.18</v>
       </c>
       <c r="E31">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>499.69</v>
       </c>
       <c r="G31" t="s">
         <v>2</v>
       </c>
       <c r="H31">
-        <f>B31</f>
+        <f t="shared" ref="H31:K32" si="11">B31</f>
         <v>976.14</v>
       </c>
       <c r="I31">
-        <f>C31</f>
+        <f t="shared" si="11"/>
         <v>737.69</v>
       </c>
       <c r="J31">
-        <f>D31</f>
-        <v>613.53</v>
+        <f t="shared" si="11"/>
+        <v>666.18</v>
       </c>
       <c r="K31">
-        <f>E31</f>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>499.69</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1185,35 +1186,35 @@
         <v>8</v>
       </c>
       <c r="C32">
-        <f t="shared" ref="C32:E32" si="6">C20</f>
+        <f t="shared" ref="C32:E32" si="12">C20</f>
         <v>27.07</v>
       </c>
       <c r="D32">
-        <f t="shared" si="6"/>
-        <v>-5.17</v>
+        <f t="shared" si="12"/>
+        <v>20.88</v>
       </c>
       <c r="E32">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>23.09</v>
       </c>
       <c r="G32" t="s">
         <v>3</v>
       </c>
       <c r="H32">
-        <f>B32</f>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="I32">
-        <f>C32</f>
+        <f t="shared" si="11"/>
         <v>27.07</v>
       </c>
       <c r="J32">
-        <f>D32</f>
-        <v>-5.17</v>
+        <f t="shared" si="11"/>
+        <v>20.88</v>
       </c>
       <c r="K32">
-        <f>E32</f>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>23.09</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1230,11 +1231,11 @@
       </c>
       <c r="D33">
         <f>D31*2+D32*LN(24*24*2)</f>
-        <v>1190.6153524707072</v>
+        <v>1479.5484410854217</v>
       </c>
       <c r="E33">
         <f>E31*2+E32*LN(24*24*2)</f>
-        <v>0</v>
+        <v>1162.1472942845974</v>
       </c>
       <c r="G33" t="s">
         <v>1</v>
@@ -1244,16 +1245,16 @@
         <v>1968.28</v>
       </c>
       <c r="I33">
-        <f t="shared" ref="I33:K33" si="7">I31*2+I32*2</f>
+        <f t="shared" ref="I33:K33" si="13">I31*2+I32*2</f>
         <v>1529.5200000000002</v>
       </c>
       <c r="J33">
-        <f t="shared" si="7"/>
-        <v>1216.72</v>
+        <f t="shared" si="13"/>
+        <v>1374.12</v>
       </c>
       <c r="K33">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1045.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished WeiSSVM real data, started on HTLP
</commit_message>
<xml_diff>
--- a/Data/C_BIC_and_AIC_new.xlsx
+++ b/Data/C_BIC_and_AIC_new.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\Documents\GitHub\Master-Thesis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEE1FD8-39FF-4C42-92DB-691A319F0A90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3BE48D-0AE5-4488-8B2D-C9C4C07F96A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{8B4AF45F-4553-42B7-ADB3-4705C4B01884}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{8B4AF45F-4553-42B7-ADB3-4705C4B01884}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="WeiSSVM" sheetId="1" r:id="rId1"/>
+    <sheet name="HTLP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="9">
   <si>
     <t>BIC</t>
   </si>
@@ -413,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149882FA-BBD9-4342-82D0-ADAD67F3F862}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1260,4 +1261,809 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D4C18F-50C8-4515-87A2-FB5916D67B55}">
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>878.13</v>
+      </c>
+      <c r="C3">
+        <v>727.78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:K4" si="0">B3</f>
+        <v>878.13</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>727.78</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>57.94</v>
+      </c>
+      <c r="C4">
+        <v>131.54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>57.94</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>131.54</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <f>B3*2+B4*LN(24*24*2)</f>
+        <v>2164.6938255023633</v>
+      </c>
+      <c r="C5">
+        <f>C3*2+C4*LN(24*24*2)</f>
+        <v>2382.8189818187925</v>
+      </c>
+      <c r="D5">
+        <f>D3*2+D4*LN(24*24*2)</f>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>E3*2+E4*LN(24*24*2)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f>H3*2+H4*2</f>
+        <v>1872.1399999999999</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:K5" si="1">I3*2+I4*2</f>
+        <v>1718.6399999999999</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>1040.3699999999999</v>
+      </c>
+      <c r="C7">
+        <v>821.15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:K8" si="2">B7</f>
+        <v>1040.3699999999999</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>821.15</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>75.78</v>
+      </c>
+      <c r="C8">
+        <v>120.88</v>
+      </c>
+      <c r="G8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>75.78</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>120.88</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <f>B7*2+B8*LN(24*24*2)</f>
+        <v>2614.9325318703673</v>
+      </c>
+      <c r="C9">
+        <f>C7*2+C8*LN(24*24*2)</f>
+        <v>2494.4139252110053</v>
+      </c>
+      <c r="D9">
+        <f>D7*2+D8*LN(24*24*2)</f>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f>E7*2+E8*LN(24*24*2)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f>H7*2+H8*2</f>
+        <v>2232.2999999999997</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ref="I9:K9" si="3">I7*2+I8*2</f>
+        <v>1884.06</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>958.24</v>
+      </c>
+      <c r="C15">
+        <v>1337.51</v>
+      </c>
+      <c r="G15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15:K16" si="4">B15</f>
+        <v>958.24</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
+        <v>1337.51</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>106.5</v>
+      </c>
+      <c r="C16">
+        <v>65.67</v>
+      </c>
+      <c r="G16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>106.5</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="4"/>
+        <v>65.67</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <f>B15*2+B16*LN(24*24*2)</f>
+        <v>2667.2256405937469</v>
+      </c>
+      <c r="C17">
+        <f>C15*2+C16*LN(24*24*2)</f>
+        <v>3137.9445654252709</v>
+      </c>
+      <c r="D17">
+        <f>D15*2+D16*LN(24*24*2)</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>E15*2+E16*LN(24*24*2)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <f>H15*2+H16*2</f>
+        <v>2129.48</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17:K17" si="5">I15*2+I16*2</f>
+        <v>2806.36</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>972.5</v>
+      </c>
+      <c r="C19">
+        <v>1326.86</v>
+      </c>
+      <c r="G19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ref="H19:K20" si="6">B19</f>
+        <v>972.5</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="6"/>
+        <v>1326.86</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>6.5</v>
+      </c>
+      <c r="C20">
+        <v>38.909999999999997</v>
+      </c>
+      <c r="G20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="6"/>
+        <v>6.5</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="6"/>
+        <v>38.909999999999997</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <f>B19*2+B20*LN(24*24*2)</f>
+        <v>1990.8201564681628</v>
+      </c>
+      <c r="C21">
+        <f>C19*2+C20*LN(24*24*2)</f>
+        <v>2928.0065058732644</v>
+      </c>
+      <c r="D21">
+        <f>D19*2+D20*LN(24*24*2)</f>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f>E19*2+E20*LN(24*24*2)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <f>H19*2+H20*2</f>
+        <v>1958</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ref="I21:K21" si="7">I19*2+I20*2</f>
+        <v>2731.54</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+      <c r="K26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <f>B3</f>
+        <v>878.13</v>
+      </c>
+      <c r="C27">
+        <f>C3</f>
+        <v>727.78</v>
+      </c>
+      <c r="D27">
+        <f>D3</f>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f>E3</f>
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ref="H27:K28" si="8">B27</f>
+        <v>878.13</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="8"/>
+        <v>727.78</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <f>B16</f>
+        <v>106.5</v>
+      </c>
+      <c r="C28">
+        <f>C16</f>
+        <v>65.67</v>
+      </c>
+      <c r="D28">
+        <f>D16</f>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f>E16</f>
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="8"/>
+        <v>106.5</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="8"/>
+        <v>65.67</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <f>B27*2+B28*LN(24*24*2)</f>
+        <v>2507.0056405937466</v>
+      </c>
+      <c r="C29">
+        <f>C27*2+C28*LN(24*24*2)</f>
+        <v>1918.4845654252708</v>
+      </c>
+      <c r="D29">
+        <f>D27*2+D28*LN(24*24*2)</f>
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <f>E27*2+E28*LN(24*24*2)</f>
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <f>H27*2+H28*2</f>
+        <v>1969.26</v>
+      </c>
+      <c r="I29">
+        <f t="shared" ref="I29:K29" si="9">I27*2+I28*2</f>
+        <v>1586.8999999999999</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <f>B7</f>
+        <v>1040.3699999999999</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31:E31" si="10">C7</f>
+        <v>821.15</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>2</v>
+      </c>
+      <c r="H31">
+        <f t="shared" ref="H31:K32" si="11">B31</f>
+        <v>1040.3699999999999</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="11"/>
+        <v>821.15</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <f>B20</f>
+        <v>6.5</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:E32" si="12">C20</f>
+        <v>38.909999999999997</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="11"/>
+        <v>6.5</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="11"/>
+        <v>38.909999999999997</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <f>B31*2+B32*LN(24*24*2)</f>
+        <v>2126.5601564681629</v>
+      </c>
+      <c r="C33">
+        <f>C31*2+C32*LN(24*24*2)</f>
+        <v>1916.5865058732645</v>
+      </c>
+      <c r="D33">
+        <f>D31*2+D32*LN(24*24*2)</f>
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <f>E31*2+E32*LN(24*24*2)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <f>H31*2+H32*2</f>
+        <v>2093.7399999999998</v>
+      </c>
+      <c r="I33">
+        <f t="shared" ref="I33:K33" si="13">I31*2+I32*2</f>
+        <v>1720.12</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
More on real data with HTLP and sample/vector windrose plots
</commit_message>
<xml_diff>
--- a/Data/C_BIC_and_AIC_new.xlsx
+++ b/Data/C_BIC_and_AIC_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\Documents\GitHub\Master-Thesis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3BE48D-0AE5-4488-8B2D-C9C4C07F96A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CEA49A-DEF6-4737-AA2E-EBB46DB8E559}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{8B4AF45F-4553-42B7-ADB3-4705C4B01884}"/>
   </bookViews>
@@ -1268,7 +1268,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1329,6 +1329,9 @@
       <c r="C3">
         <v>727.78</v>
       </c>
+      <c r="E3">
+        <v>440.16</v>
+      </c>
       <c r="G3" t="s">
         <v>2</v>
       </c>
@@ -1346,7 +1349,7 @@
       </c>
       <c r="K3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>440.16</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1358,6 +1361,9 @@
       </c>
       <c r="C4">
         <v>131.54</v>
+      </c>
+      <c r="E4">
+        <v>263.79000000000002</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
@@ -1376,7 +1382,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>263.79000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1397,7 +1403,7 @@
       </c>
       <c r="E5">
         <f>E3*2+E4*LN(24*24*2)</f>
-        <v>0</v>
+        <v>2739.8429345748773</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
@@ -1416,7 +1422,7 @@
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1407.9</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1436,6 +1442,12 @@
       </c>
       <c r="C7">
         <v>821.15</v>
+      </c>
+      <c r="D7">
+        <v>589.66999999999996</v>
+      </c>
+      <c r="E7">
+        <v>494.82</v>
       </c>
       <c r="G7" t="s">
         <v>2</v>
@@ -1450,11 +1462,11 @@
       </c>
       <c r="J7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>589.66999999999996</v>
       </c>
       <c r="K7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>494.82</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1466,6 +1478,12 @@
       </c>
       <c r="C8">
         <v>120.88</v>
+      </c>
+      <c r="D8">
+        <v>205.92</v>
+      </c>
+      <c r="E8">
+        <v>232.18</v>
       </c>
       <c r="G8" t="s">
         <v>3</v>
@@ -1480,11 +1498,11 @@
       </c>
       <c r="J8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>205.92</v>
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>232.18</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1501,11 +1519,11 @@
       </c>
       <c r="D9">
         <f>D7*2+D8*LN(24*24*2)</f>
-        <v>0</v>
+        <v>2630.9225569114014</v>
       </c>
       <c r="E9">
         <f>E7*2+E8*LN(24*24*2)</f>
-        <v>0</v>
+        <v>2626.3359890427801</v>
       </c>
       <c r="G9" t="s">
         <v>1</v>
@@ -1520,11 +1538,11 @@
       </c>
       <c r="J9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1591.1799999999998</v>
       </c>
       <c r="K9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1577,6 +1595,9 @@
       <c r="C15">
         <v>1337.51</v>
       </c>
+      <c r="E15">
+        <v>1821.15</v>
+      </c>
       <c r="G15" t="s">
         <v>2</v>
       </c>
@@ -1594,7 +1615,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1821.15</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1606,6 +1627,9 @@
       </c>
       <c r="C16">
         <v>65.67</v>
+      </c>
+      <c r="E16">
+        <v>32.659999999999997</v>
       </c>
       <c r="G16" t="s">
         <v>3</v>
@@ -1624,7 +1648,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>32.659999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1645,7 +1669,7 @@
       </c>
       <c r="E17">
         <f>E15*2+E16*LN(24*24*2)</f>
-        <v>0</v>
+        <v>3872.5286631154158</v>
       </c>
       <c r="G17" t="s">
         <v>1</v>
@@ -1664,7 +1688,7 @@
       </c>
       <c r="K17">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3707.6200000000003</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1684,6 +1708,12 @@
       </c>
       <c r="C19">
         <v>1326.86</v>
+      </c>
+      <c r="D19">
+        <v>1597.37</v>
+      </c>
+      <c r="E19">
+        <v>1796.33</v>
       </c>
       <c r="G19" t="s">
         <v>2</v>
@@ -1698,11 +1728,11 @@
       </c>
       <c r="J19">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1597.37</v>
       </c>
       <c r="K19">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1796.33</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1714,6 +1744,12 @@
       </c>
       <c r="C20">
         <v>38.909999999999997</v>
+      </c>
+      <c r="D20">
+        <v>-19.940000000000001</v>
+      </c>
+      <c r="E20">
+        <v>-11.33</v>
       </c>
       <c r="G20" t="s">
         <v>3</v>
@@ -1728,11 +1764,11 @@
       </c>
       <c r="J20">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-19.940000000000001</v>
       </c>
       <c r="K20">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-11.33</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1749,11 +1785,11 @@
       </c>
       <c r="D21">
         <f>D19*2+D20*LN(24*24*2)</f>
-        <v>0</v>
+        <v>3054.1778584653584</v>
       </c>
       <c r="E21">
         <f>E19*2+E20*LN(24*24*2)</f>
-        <v>0</v>
+        <v>3512.7919426485714</v>
       </c>
       <c r="G21" t="s">
         <v>1</v>
@@ -1768,11 +1804,11 @@
       </c>
       <c r="J21">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3154.8599999999997</v>
       </c>
       <c r="K21">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3570</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1833,7 +1869,7 @@
       </c>
       <c r="E27">
         <f>E3</f>
-        <v>0</v>
+        <v>440.16</v>
       </c>
       <c r="G27" t="s">
         <v>2</v>
@@ -1852,7 +1888,7 @@
       </c>
       <c r="K27">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>440.16</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1873,7 +1909,7 @@
       </c>
       <c r="E28">
         <f>E16</f>
-        <v>0</v>
+        <v>32.659999999999997</v>
       </c>
       <c r="G28" t="s">
         <v>3</v>
@@ -1892,7 +1928,7 @@
       </c>
       <c r="K28">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>32.659999999999997</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1913,7 +1949,7 @@
       </c>
       <c r="E29">
         <f>E27*2+E28*LN(24*24*2)</f>
-        <v>0</v>
+        <v>1110.5486631154156</v>
       </c>
       <c r="G29" t="s">
         <v>1</v>
@@ -1932,7 +1968,7 @@
       </c>
       <c r="K29">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>945.6400000000001</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1957,11 +1993,11 @@
       </c>
       <c r="D31">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>589.66999999999996</v>
       </c>
       <c r="E31">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>494.82</v>
       </c>
       <c r="G31" t="s">
         <v>2</v>
@@ -1976,11 +2012,11 @@
       </c>
       <c r="J31">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>589.66999999999996</v>
       </c>
       <c r="K31">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>494.82</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1997,11 +2033,11 @@
       </c>
       <c r="D32">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-19.940000000000001</v>
       </c>
       <c r="E32">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-11.33</v>
       </c>
       <c r="G32" t="s">
         <v>3</v>
@@ -2016,11 +2052,11 @@
       </c>
       <c r="J32">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-19.940000000000001</v>
       </c>
       <c r="K32">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-11.33</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2037,11 +2073,11 @@
       </c>
       <c r="D33">
         <f>D31*2+D32*LN(24*24*2)</f>
-        <v>0</v>
+        <v>1038.7778584653586</v>
       </c>
       <c r="E33">
         <f>E31*2+E32*LN(24*24*2)</f>
-        <v>0</v>
+        <v>909.77194264857133</v>
       </c>
       <c r="G33" t="s">
         <v>1</v>
@@ -2056,11 +2092,11 @@
       </c>
       <c r="J33">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1139.4599999999998</v>
       </c>
       <c r="K33">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>966.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>